<commit_message>
Implementación de múltiples scripts para mejorar la compatibilidad y la experiencia de usuario en macOS. Se añadieron scripts específicos para macOS, correcciones de visualización, y un enfoque alternativo utilizando PyObjC. Se mejoraron las configuraciones de entorno para evitar problemas de tema oscuro y se implementaron métodos automatizados para ejecutar la aplicación con diferentes configuraciones. Se creó un script de prueba para verificar la funcionalidad básica de Tkinter en macOS. Además, se optimizó la interfaz de usuario y se mejoró la gestión de errores en la generación de etiquetas.
</commit_message>
<xml_diff>
--- a/etiqueta_generator/data.xlsx
+++ b/etiqueta_generator/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/nvme/workspace/jolg/etiquetas/etiqueta_generator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4482EF4F-D4CE-0B4D-8DA2-03249B9CDA9E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939721AF-A1F4-F84F-AFA4-8D8D4AF7875E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{31FF99D6-B8C2-6847-9786-4EC179471A8B}"/>
   </bookViews>
@@ -867,6 +867,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="28.83203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">

</xml_diff>